<commit_message>
Update layout, global layout and 2 variable plots
</commit_message>
<xml_diff>
--- a/Data/exemplo1ANCOVA.xlsx
+++ b/Data/exemplo1ANCOVA.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wfrocha\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\PycharmProjects\VDI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D902F72C-7CC0-4C50-91C1-100B41E522C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="19944" windowHeight="10956" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,13 +37,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="8">
   <si>
-    <t>velocity_ratio</t>
-  </si>
-  <si>
     <t>Err</t>
-  </si>
-  <si>
-    <t>oil</t>
   </si>
   <si>
     <t>gas</t>
@@ -59,11 +54,17 @@
   <si>
     <t>Siptech_90_cSt</t>
   </si>
+  <si>
+    <t>Fluido</t>
+  </si>
+  <si>
+    <t>Velocity ratio</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -411,30 +412,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="14.85546875" style="1" customWidth="1"/>
+    <col min="1" max="3" width="14.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1.16001</v>
       </c>
@@ -442,10 +441,10 @@
         <v>1.2102442560017299</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1.160048</v>
       </c>
@@ -453,10 +452,10 @@
         <v>1.2335948143222999</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1.1588830000000001</v>
       </c>
@@ -464,10 +463,10 @@
         <v>1.22228909371821</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1.1588609999999999</v>
       </c>
@@ -475,10 +474,10 @@
         <v>1.2521636205579201</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1.158976</v>
       </c>
@@ -486,10 +485,10 @@
         <v>1.24735348451207</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1.166736</v>
       </c>
@@ -497,10 +496,10 @@
         <v>1.2024100928510799</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1.1656010000000001</v>
       </c>
@@ -508,10 +507,10 @@
         <v>1.2548694302471199</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1.1664570000000001</v>
       </c>
@@ -519,10 +518,10 @@
         <v>1.2766953528075999</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1.165694</v>
       </c>
@@ -530,10 +529,10 @@
         <v>1.1835657829522901</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>1.167259</v>
       </c>
@@ -541,10 +540,10 @@
         <v>1.22302192934158</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>1.1717569999999999</v>
       </c>
@@ -552,10 +551,10 @@
         <v>1.3391491994038101</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>1.1714059999999999</v>
       </c>
@@ -563,10 +562,10 @@
         <v>1.2837848397462499</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>1.1725719999999999</v>
       </c>
@@ -574,10 +573,10 @@
         <v>1.33592071044466</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>1.1723600000000001</v>
       </c>
@@ -585,10 +584,10 @@
         <v>1.3166793497244</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>1.1699550000000001</v>
       </c>
@@ -596,10 +595,10 @@
         <v>1.25776288997055</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>1.179902</v>
       </c>
@@ -607,10 +606,10 @@
         <v>1.37675901727959</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>1.1792910000000001</v>
       </c>
@@ -618,10 +617,10 @@
         <v>1.3285275381733901</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>1.182134</v>
       </c>
@@ -629,10 +628,10 @@
         <v>1.3556940216711799</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>1.1815100000000001</v>
       </c>
@@ -640,10 +639,10 @@
         <v>1.3552924823078401</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>1.183206</v>
       </c>
@@ -651,10 +650,10 @@
         <v>1.3222490411299901</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>1.189686</v>
       </c>
@@ -662,10 +661,10 @@
         <v>1.4733913525596301</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>1.1873400000000001</v>
       </c>
@@ -673,10 +672,10 @@
         <v>1.3568759703675499</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>1.189964</v>
       </c>
@@ -684,10 +683,10 @@
         <v>1.4018463858055199</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>1.1906859999999999</v>
       </c>
@@ -695,10 +694,10 @@
         <v>1.3865631146245601</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>1.190053</v>
       </c>
@@ -706,10 +705,10 @@
         <v>1.4040378911585301</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>1.193986</v>
       </c>
@@ -717,10 +716,10 @@
         <v>1.3544567629178299</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>1.1985170000000001</v>
       </c>
@@ -728,10 +727,10 @@
         <v>1.3916007379853399</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>1.1939280000000001</v>
       </c>
@@ -739,10 +738,10 @@
         <v>1.3976532429240101</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>1.1937359999999999</v>
       </c>
@@ -750,10 +749,10 @@
         <v>1.41874323149105</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>1.1941310000000001</v>
       </c>
@@ -761,10 +760,10 @@
         <v>1.38090673551719</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>1.1972739999999999</v>
       </c>
@@ -772,10 +771,10 @@
         <v>1.42120735872112</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>1.185119</v>
       </c>
@@ -783,10 +782,10 @@
         <v>1.29603447153512</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>1.1837519999999999</v>
       </c>
@@ -794,10 +793,10 @@
         <v>1.3083397981052101</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>1.18652</v>
       </c>
@@ -805,10 +804,10 @@
         <v>1.28525936576557</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>1.1833750000000001</v>
       </c>
@@ -816,10 +815,10 @@
         <v>1.28523455520945</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>1.181468</v>
       </c>
@@ -827,10 +826,10 @@
         <v>1.2934773768716701</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>1.172396</v>
       </c>
@@ -838,10 +837,10 @@
         <v>1.1915808457291801</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>1.173597</v>
       </c>
@@ -849,10 +848,10 @@
         <v>1.2591924430229999</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>1.1720759999999999</v>
       </c>
@@ -860,10 +859,10 @@
         <v>1.22183495773867</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>1.1741569999999999</v>
       </c>
@@ -871,10 +870,10 @@
         <v>1.23579953175234</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>1.1736230000000001</v>
       </c>
@@ -882,10 +881,10 @@
         <v>1.2164283233265201</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>1.1633500000000001</v>
       </c>
@@ -893,10 +892,10 @@
         <v>1.1788877654941099</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>1.1651020000000001</v>
       </c>
@@ -904,10 +903,10 @@
         <v>1.1695061931728901</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>1.160957</v>
       </c>
@@ -915,10 +914,10 @@
         <v>1.2073480133665599</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>1.16025</v>
       </c>
@@ -926,10 +925,10 @@
         <v>1.1788108564717299</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>1.159707</v>
       </c>
@@ -937,10 +936,10 @@
         <v>1.18996685781477</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>1.14839</v>
       </c>
@@ -948,10 +947,10 @@
         <v>1.1725113336628501</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>1.150247</v>
       </c>
@@ -959,10 +958,10 @@
         <v>1.1638402311795599</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>1.1487560000000001</v>
       </c>
@@ -970,10 +969,10 @@
         <v>1.2101140226971401</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>1.1496919999999999</v>
       </c>
@@ -981,10 +980,10 @@
         <v>1.1653452702506599</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>1.149545</v>
       </c>
@@ -992,10 +991,10 @@
         <v>1.12667208682159</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>1.1452279999999999</v>
       </c>
@@ -1003,10 +1002,10 @@
         <v>1.10137448507804</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>1.144091</v>
       </c>
@@ -1014,10 +1013,10 @@
         <v>1.0691367713900699</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>1.1452690000000001</v>
       </c>
@@ -1025,10 +1024,10 @@
         <v>1.1064590620135</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>1.1449590000000001</v>
       </c>
@@ -1036,10 +1035,10 @@
         <v>1.11311286741376</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>1.215498</v>
       </c>
@@ -1047,10 +1046,10 @@
         <v>1.6673500792806</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>1.2158409999999999</v>
       </c>
@@ -1058,10 +1057,10 @@
         <v>1.6315688972259199</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>1.2152989999999999</v>
       </c>
@@ -1069,10 +1068,10 @@
         <v>1.6969553578976599</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>1.215441</v>
       </c>
@@ -1080,10 +1079,10 @@
         <v>1.60317395961349</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>1.215098</v>
       </c>
@@ -1091,10 +1090,10 @@
         <v>1.6350481191623101</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>1.211309</v>
       </c>
@@ -1102,10 +1101,10 @@
         <v>1.5917449252524201</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>1.211921</v>
       </c>
@@ -1113,10 +1112,10 @@
         <v>1.5885316889921599</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>1.210904</v>
       </c>
@@ -1124,10 +1123,10 @@
         <v>1.61616847707696</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>1.2110019999999999</v>
       </c>
@@ -1135,10 +1134,10 @@
         <v>1.6259453520407801</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>1.2127049999999999</v>
       </c>
@@ -1146,10 +1145,10 @@
         <v>1.60789429091537</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>1.2041120000000001</v>
       </c>
@@ -1157,10 +1156,10 @@
         <v>1.5018246437581899</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>1.2038059999999999</v>
       </c>
@@ -1168,10 +1167,10 @@
         <v>1.52242168380552</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>1.204501</v>
       </c>
@@ -1179,10 +1178,10 @@
         <v>1.5070795740257299</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>1.2036880000000001</v>
       </c>
@@ -1190,10 +1189,10 @@
         <v>1.46874314981706</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>1.2023440000000001</v>
       </c>
@@ -1201,10 +1200,10 @@
         <v>1.46071220296548</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>1.1984239999999999</v>
       </c>
@@ -1212,10 +1211,10 @@
         <v>1.3980778646726599</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>1.1973529999999999</v>
       </c>
@@ -1223,10 +1222,10 @@
         <v>1.4185854194743499</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>1.1990080000000001</v>
       </c>
@@ -1234,10 +1233,10 @@
         <v>1.4285048961753399</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>1.1987989999999999</v>
       </c>
@@ -1245,10 +1244,10 @@
         <v>1.4601423986688999</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>1.1972160000000001</v>
       </c>
@@ -1256,10 +1255,10 @@
         <v>1.3997373153095101</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>1.1879459999999999</v>
       </c>
@@ -1267,10 +1266,10 @@
         <v>1.3057597447561899</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>1.1886369999999999</v>
       </c>
@@ -1278,10 +1277,10 @@
         <v>1.3285742355910799</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>1.188823</v>
       </c>
@@ -1289,10 +1288,10 @@
         <v>1.3125735916775301</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>1.189343</v>
       </c>
@@ -1300,10 +1299,10 @@
         <v>1.3203659488464401</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>1.1879679999999999</v>
       </c>
@@ -1311,10 +1310,10 @@
         <v>1.28427803418105</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>1.23577</v>
       </c>
@@ -1322,10 +1321,10 @@
         <v>1.7253420918159501</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>1.234901</v>
       </c>
@@ -1333,10 +1332,10 @@
         <v>1.7569711781815101</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>1.235185</v>
       </c>
@@ -1344,10 +1343,10 @@
         <v>1.76960704573099</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>1.2329760000000001</v>
       </c>
@@ -1355,10 +1354,10 @@
         <v>1.73889701926934</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>1.236408</v>
       </c>
@@ -1366,10 +1365,10 @@
         <v>1.75602518105229</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>1.2234579999999999</v>
       </c>
@@ -1377,10 +1376,10 @@
         <v>1.8388803699463001</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>1.2237279999999999</v>
       </c>
@@ -1388,10 +1387,10 @@
         <v>1.7791843377962899</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>1.2236119999999999</v>
       </c>
@@ -1399,10 +1398,10 @@
         <v>1.6542685005132001</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>1.2280899999999999</v>
       </c>
@@ -1410,10 +1409,10 @@
         <v>1.69905902339759</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>1.2269300000000001</v>
       </c>
@@ -1421,10 +1420,10 @@
         <v>1.76520698119996</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>1.2154560000000001</v>
       </c>
@@ -1432,10 +1431,10 @@
         <v>1.6180976772464599</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>1.2150780000000001</v>
       </c>
@@ -1443,10 +1442,10 @@
         <v>1.6354576745282901</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>1.2133100000000001</v>
       </c>
@@ -1454,10 +1453,10 @@
         <v>1.6608462697336801</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>1.211929</v>
       </c>
@@ -1465,10 +1464,10 @@
         <v>1.57175990018752</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>1.211103</v>
       </c>
@@ -1476,10 +1475,10 @@
         <v>1.56873155242542</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>1.206502</v>
       </c>
@@ -1487,10 +1486,10 @@
         <v>1.51236417601684</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>1.2068270000000001</v>
       </c>
@@ -1498,10 +1497,10 @@
         <v>1.5860817468592301</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>1.20892</v>
       </c>
@@ -1509,10 +1508,10 @@
         <v>1.5069688702070601</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>1.208461</v>
       </c>
@@ -1520,10 +1519,10 @@
         <v>1.57463742767602</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>1.2089380000000001</v>
       </c>
@@ -1531,10 +1530,10 @@
         <v>1.4215585672786899</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>1.203147</v>
       </c>
@@ -1542,10 +1541,10 @@
         <v>1.45664599037029</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>1.2048080000000001</v>
       </c>
@@ -1553,10 +1552,10 @@
         <v>1.49224384775352</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>1.2033929999999999</v>
       </c>
@@ -1564,10 +1563,10 @@
         <v>1.48223668494857</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>1.2039029999999999</v>
       </c>
@@ -1575,10 +1574,10 @@
         <v>1.4444561634917299</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>1.2028779999999999</v>
       </c>
@@ -1586,10 +1585,10 @@
         <v>1.4354699417905099</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>1.2013480000000001</v>
       </c>
@@ -1597,10 +1596,10 @@
         <v>1.3828888074416501</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>1.199921</v>
       </c>
@@ -1608,10 +1607,10 @@
         <v>1.4065977816138799</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>1.2018690000000001</v>
       </c>
@@ -1619,10 +1618,10 @@
         <v>1.4411321317538699</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>1.199106</v>
       </c>
@@ -1630,10 +1629,10 @@
         <v>1.3624672241504101</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>1.1995960000000001</v>
       </c>
@@ -1641,10 +1640,10 @@
         <v>1.3465591693615899</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>1.1966829999999999</v>
       </c>
@@ -1652,10 +1651,10 @@
         <v>1.32412040937372</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>1.1946209999999999</v>
       </c>
@@ -1663,10 +1662,10 @@
         <v>1.3560840957820599</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>1.1940489999999999</v>
       </c>
@@ -1674,10 +1673,10 @@
         <v>1.3249404100698099</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>1.19432</v>
       </c>
@@ -1685,10 +1684,10 @@
         <v>1.35875680821185</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>1.195271</v>
       </c>
@@ -1696,10 +1695,10 @@
         <v>1.2876052244948899</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>1.2360660000000001</v>
       </c>
@@ -1707,10 +1706,10 @@
         <v>1.7648030299117401</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>1.2308870000000001</v>
       </c>
@@ -1718,10 +1717,10 @@
         <v>1.7136881770344301</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>1.235114</v>
       </c>
@@ -1729,10 +1728,10 @@
         <v>1.7922194080587801</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>1.2347379999999999</v>
       </c>
@@ -1740,10 +1739,10 @@
         <v>1.7589502835803501</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>1.2388349999999999</v>
       </c>
@@ -1751,10 +1750,10 @@
         <v>1.6966854965523801</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>1.2274259999999999</v>
       </c>
@@ -1762,10 +1761,10 @@
         <v>1.71869198752188</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>1.224172</v>
       </c>
@@ -1773,10 +1772,10 @@
         <v>1.6990607150805299</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>1.2252700000000001</v>
       </c>
@@ -1784,10 +1783,10 @@
         <v>1.69733035692887</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>1.2263520000000001</v>
       </c>
@@ -1795,10 +1794,10 @@
         <v>1.70413945222911</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>1.224448</v>
       </c>
@@ -1806,10 +1805,10 @@
         <v>1.67325629850567</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>1.2188159999999999</v>
       </c>
@@ -1817,10 +1816,10 @@
         <v>1.6735686223284001</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>1.218656</v>
       </c>
@@ -1828,10 +1827,10 @@
         <v>1.64991724391118</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>1.2182809999999999</v>
       </c>
@@ -1839,10 +1838,10 @@
         <v>1.6568710490810199</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>1.219106</v>
       </c>
@@ -1850,10 +1849,10 @@
         <v>1.6568710490810199</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>1.21855</v>
       </c>
@@ -1861,10 +1860,10 @@
         <v>1.6536394748748999</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>1.213212</v>
       </c>
@@ -1872,10 +1871,10 @@
         <v>1.5857006521311501</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>1.211587</v>
       </c>
@@ -1883,10 +1882,10 @@
         <v>1.4229570178677899</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>1.2100599999999999</v>
       </c>
@@ -1894,10 +1893,10 @@
         <v>1.59776249476381</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>1.2119949999999999</v>
       </c>
@@ -1905,10 +1904,10 @@
         <v>1.5624167409714</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>1.213606</v>
       </c>
@@ -1916,10 +1915,11 @@
         <v>1.67707867958099</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>